<commit_message>
Add readme file, adjust nodes' x, y coordinates, add gis layer, and add input file for gams code
</commit_message>
<xml_diff>
--- a/data/Gas_Transmission/Gas_Trans.xlsx
+++ b/data/Gas_Transmission/Gas_Trans.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\Adam_Project\GAMS_Code\GAS\Belgium\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\Apps\demos\data\Gas_Transmission\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="14400" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="14400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="network" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1869" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="115">
   <si>
     <t>Name</t>
   </si>
@@ -214,127 +214,7 @@
     <t>X</t>
   </si>
   <si>
-    <t>497.0000000000</t>
-  </si>
-  <si>
-    <t>439.0000000000</t>
-  </si>
-  <si>
     <t>city</t>
-  </si>
-  <si>
-    <t>549.0000000000</t>
-  </si>
-  <si>
-    <t>290.0000000000</t>
-  </si>
-  <si>
-    <t>788.0000000000</t>
-  </si>
-  <si>
-    <t>681.0000000000</t>
-  </si>
-  <si>
-    <t>760.0000000000</t>
-  </si>
-  <si>
-    <t>401.0000000000</t>
-  </si>
-  <si>
-    <t>430.0000000000</t>
-  </si>
-  <si>
-    <t>522.0000000000</t>
-  </si>
-  <si>
-    <t>338.0000000000</t>
-  </si>
-  <si>
-    <t>298.0000000000</t>
-  </si>
-  <si>
-    <t>346.0000000000</t>
-  </si>
-  <si>
-    <t>259.0000000000</t>
-  </si>
-  <si>
-    <t>443.0000000000</t>
-  </si>
-  <si>
-    <t>320.0000000000</t>
-  </si>
-  <si>
-    <t>764.0000000000</t>
-  </si>
-  <si>
-    <t>396.0000000000</t>
-  </si>
-  <si>
-    <t>616.0000000000</t>
-  </si>
-  <si>
-    <t>221.0000000000</t>
-  </si>
-  <si>
-    <t>427.0000000000</t>
-  </si>
-  <si>
-    <t>462.0000000000</t>
-  </si>
-  <si>
-    <t>611.0000000000</t>
-  </si>
-  <si>
-    <t>496.0000000000</t>
-  </si>
-  <si>
-    <t>468.0000000000</t>
-  </si>
-  <si>
-    <t>456.0000000000</t>
-  </si>
-  <si>
-    <t>840.0000000000</t>
-  </si>
-  <si>
-    <t>720.0000000000</t>
-  </si>
-  <si>
-    <t>695.0000000000</t>
-  </si>
-  <si>
-    <t>533.0000000000</t>
-  </si>
-  <si>
-    <t>750.0000000000</t>
-  </si>
-  <si>
-    <t>453.0000000000</t>
-  </si>
-  <si>
-    <t>687.0000000000</t>
-  </si>
-  <si>
-    <t>480.0000000000</t>
-  </si>
-  <si>
-    <t>690.0000000000</t>
-  </si>
-  <si>
-    <t>434.0000000000</t>
-  </si>
-  <si>
-    <t>332.0000000000</t>
-  </si>
-  <si>
-    <t>235.0000000000</t>
-  </si>
-  <si>
-    <t>385.0000000000</t>
-  </si>
-  <si>
-    <t>301.0000000000</t>
   </si>
   <si>
     <t>link</t>
@@ -885,7 +765,7 @@
         <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>153</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -992,76 +872,76 @@
         <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>119</v>
+        <v>79</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.25">
@@ -1069,76 +949,76 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="J2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="L2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="N2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="P2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="R2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="T2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="V2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="X2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="Z2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AB2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AD2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AF2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AH2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AJ2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AL2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AN2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AP2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AR2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AT2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AV2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.25">
@@ -4272,8 +4152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4345,10 +4225,10 @@
         <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>151</v>
+        <v>111</v>
       </c>
       <c r="J2" t="s">
-        <v>145</v>
+        <v>105</v>
       </c>
       <c r="K2" t="s">
         <v>24</v>
@@ -4358,14 +4238,14 @@
       <c r="A3" t="s">
         <v>37</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>429369</v>
+      </c>
+      <c r="C3">
+        <v>6495706</v>
+      </c>
+      <c r="D3" t="s">
         <v>58</v>
-      </c>
-      <c r="C3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" t="s">
-        <v>60</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -4393,14 +4273,14 @@
       <c r="A4" t="s">
         <v>38</v>
       </c>
-      <c r="B4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" t="s">
-        <v>62</v>
+      <c r="B4">
+        <v>493318</v>
+      </c>
+      <c r="C4">
+        <v>6671775</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E4" s="1">
         <v>-900</v>
@@ -4428,14 +4308,14 @@
       <c r="A5" t="s">
         <v>39</v>
       </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>64</v>
+      <c r="B5">
+        <v>648199</v>
+      </c>
+      <c r="C5">
+        <v>6392646</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E5" s="1">
         <v>-900</v>
@@ -4463,14 +4343,14 @@
       <c r="A6" t="s">
         <v>40</v>
       </c>
-      <c r="B6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" t="s">
-        <v>66</v>
+      <c r="B6">
+        <v>638194</v>
+      </c>
+      <c r="C6">
+        <v>6576140</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
@@ -4498,14 +4378,14 @@
       <c r="A7" t="s">
         <v>41</v>
       </c>
-      <c r="B7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" t="s">
-        <v>68</v>
+      <c r="B7">
+        <v>434192</v>
+      </c>
+      <c r="C7">
+        <v>6508653</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E7" s="1">
         <v>-900</v>
@@ -4533,14 +4413,14 @@
       <c r="A8" t="s">
         <v>42</v>
       </c>
-      <c r="B8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" t="s">
-        <v>70</v>
+      <c r="B8">
+        <v>368666</v>
+      </c>
+      <c r="C8">
+        <v>6660982</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E8" s="1">
         <v>-900</v>
@@ -4568,14 +4448,14 @@
       <c r="A9" t="s">
         <v>43</v>
       </c>
-      <c r="B9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" t="s">
-        <v>72</v>
+      <c r="B9">
+        <v>359500</v>
+      </c>
+      <c r="C9">
+        <v>6670051</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
@@ -4603,14 +4483,14 @@
       <c r="A10" t="s">
         <v>44</v>
       </c>
-      <c r="B10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" t="s">
-        <v>74</v>
+      <c r="B10">
+        <v>415761</v>
+      </c>
+      <c r="C10">
+        <v>6633377</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E10" s="1">
         <v>-900</v>
@@ -4638,14 +4518,14 @@
       <c r="A11" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" t="s">
-        <v>76</v>
+      <c r="B11">
+        <v>627891</v>
+      </c>
+      <c r="C11">
+        <v>6563768</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E11" s="1">
         <v>-900</v>
@@ -4673,14 +4553,14 @@
       <c r="A12" t="s">
         <v>46</v>
       </c>
-      <c r="B12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" t="s">
-        <v>78</v>
+      <c r="B12">
+        <v>516936</v>
+      </c>
+      <c r="C12">
+        <v>6692418</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
@@ -4708,14 +4588,14 @@
       <c r="A13" t="s">
         <v>47</v>
       </c>
-      <c r="B13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" t="s">
-        <v>80</v>
+      <c r="B13">
+        <v>439995</v>
+      </c>
+      <c r="C13">
+        <v>6524528</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E13" s="1">
         <v>-900</v>
@@ -4743,14 +4623,14 @@
       <c r="A14" t="s">
         <v>48</v>
       </c>
-      <c r="B14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" t="s">
-        <v>82</v>
+      <c r="B14">
+        <v>547981</v>
+      </c>
+      <c r="C14">
+        <v>6537591</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E14" s="1">
         <v>-900</v>
@@ -4778,14 +4658,14 @@
       <c r="A15" t="s">
         <v>49</v>
       </c>
-      <c r="B15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C15" t="s">
-        <v>84</v>
+      <c r="B15">
+        <v>461688</v>
+      </c>
+      <c r="C15">
+        <v>6522264</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
@@ -4813,14 +4693,14 @@
       <c r="A16" t="s">
         <v>50</v>
       </c>
-      <c r="B16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" t="s">
-        <v>86</v>
+      <c r="B16">
+        <v>654607</v>
+      </c>
+      <c r="C16">
+        <v>6370160</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E16" s="1">
         <v>-900</v>
@@ -4848,14 +4728,14 @@
       <c r="A17" t="s">
         <v>51</v>
       </c>
-      <c r="B17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" t="s">
-        <v>88</v>
+      <c r="B17">
+        <v>586210</v>
+      </c>
+      <c r="C17">
+        <v>6494500</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
@@ -4883,14 +4763,14 @@
       <c r="A18" t="s">
         <v>52</v>
       </c>
-      <c r="B18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" t="s">
-        <v>90</v>
+      <c r="B18">
+        <v>641508</v>
+      </c>
+      <c r="C18">
+        <v>6578772</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E18" s="1">
         <v>20.344000000000001</v>
@@ -4918,14 +4798,14 @@
       <c r="A19" t="s">
         <v>53</v>
       </c>
-      <c r="B19" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" t="s">
-        <v>92</v>
+      <c r="B19">
+        <v>581029</v>
+      </c>
+      <c r="C19">
+        <v>6539330</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
@@ -4953,14 +4833,14 @@
       <c r="A20" t="s">
         <v>54</v>
       </c>
-      <c r="B20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C20" t="s">
-        <v>94</v>
+      <c r="B20">
+        <v>579118</v>
+      </c>
+      <c r="C20">
+        <v>6551332</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -4988,14 +4868,14 @@
       <c r="A21" t="s">
         <v>55</v>
       </c>
-      <c r="B21" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21" t="s">
-        <v>96</v>
+      <c r="B21">
+        <v>357870</v>
+      </c>
+      <c r="C21">
+        <v>6680229</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E21" s="1">
         <v>8.8699999999999992</v>
@@ -5023,14 +4903,14 @@
       <c r="A22" t="s">
         <v>56</v>
       </c>
-      <c r="B22" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" t="s">
-        <v>98</v>
+      <c r="B22">
+        <v>397652</v>
+      </c>
+      <c r="C22">
+        <v>6642641</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
@@ -5192,10 +5072,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>124</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
         <v>22</v>
@@ -5218,18 +5098,18 @@
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="F2" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="G2" t="s">
-        <v>145</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>37</v>
@@ -5238,7 +5118,7 @@
         <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E3" s="1">
         <v>890</v>
@@ -5252,7 +5132,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>38</v>
@@ -5261,7 +5141,7 @@
         <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E4" s="1">
         <v>590.1</v>
@@ -5275,7 +5155,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>39</v>
@@ -5284,7 +5164,7 @@
         <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E5" s="1">
         <v>315.5</v>
@@ -5298,7 +5178,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>40</v>
@@ -5307,7 +5187,7 @@
         <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E6" s="1">
         <v>890</v>
@@ -5321,7 +5201,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>40</v>
@@ -5330,7 +5210,7 @@
         <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E7" s="1">
         <v>395</v>
@@ -5344,7 +5224,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>42</v>
@@ -5353,7 +5233,7 @@
         <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E8" s="1">
         <v>890</v>
@@ -5367,7 +5247,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>43</v>
@@ -5376,7 +5256,7 @@
         <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E9" s="1">
         <v>890</v>
@@ -5390,7 +5270,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>43</v>
@@ -5399,7 +5279,7 @@
         <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E10" s="1">
         <v>890</v>
@@ -5413,7 +5293,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>44</v>
@@ -5422,7 +5302,7 @@
         <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E11" s="1">
         <v>590.1</v>
@@ -5436,7 +5316,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>45</v>
@@ -5445,7 +5325,7 @@
         <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E12" s="1">
         <v>890</v>
@@ -5459,7 +5339,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>45</v>
@@ -5468,7 +5348,7 @@
         <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E13" s="1">
         <v>395</v>
@@ -5482,7 +5362,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>46</v>
@@ -5491,7 +5371,7 @@
         <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E14" s="1">
         <v>590.1</v>
@@ -5505,7 +5385,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>47</v>
@@ -5514,7 +5394,7 @@
         <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E15" s="1">
         <v>890</v>
@@ -5528,7 +5408,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>48</v>
@@ -5537,7 +5417,7 @@
         <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E16" s="1">
         <v>890</v>
@@ -5551,7 +5431,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>49</v>
@@ -5560,7 +5440,7 @@
         <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E17" s="1">
         <v>890</v>
@@ -5574,7 +5454,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>51</v>
@@ -5583,7 +5463,7 @@
         <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E18" s="1">
         <v>315.5</v>
@@ -5597,7 +5477,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>52</v>
@@ -5606,7 +5486,7 @@
         <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="E19" s="1">
         <v>890</v>
@@ -5620,7 +5500,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>52</v>
@@ -5629,7 +5509,7 @@
         <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="E20" s="1">
         <v>395</v>
@@ -5643,7 +5523,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>53</v>
@@ -5652,7 +5532,7 @@
         <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="E21" s="1">
         <v>315.5</v>
@@ -5666,7 +5546,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>119</v>
+        <v>79</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>54</v>
@@ -5675,7 +5555,7 @@
         <v>48</v>
       </c>
       <c r="D22" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E22" s="1">
         <v>890</v>
@@ -5689,7 +5569,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>54</v>
@@ -5698,7 +5578,7 @@
         <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E23" s="1">
         <v>395.5</v>
@@ -5712,7 +5592,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>55</v>
@@ -5721,7 +5601,7 @@
         <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E24" s="1">
         <v>890</v>
@@ -5735,7 +5615,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>55</v>
@@ -5744,7 +5624,7 @@
         <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E25" s="1">
         <v>890</v>
@@ -5758,7 +5638,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>56</v>
@@ -5767,7 +5647,7 @@
         <v>49</v>
       </c>
       <c r="D26" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="E26" s="1">
         <v>890</v>
@@ -5935,7 +5815,7 @@
         <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -5947,7 +5827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -5984,7 +5864,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5998,7 +5878,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -6006,13 +5886,13 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>142</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -6020,13 +5900,13 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -6034,13 +5914,13 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>147</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6054,7 +5934,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>152</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -6062,13 +5942,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>143</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6076,13 +5956,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>135</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -6096,7 +5976,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -6110,7 +5990,7 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>133</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -6124,7 +6004,7 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -6138,7 +6018,7 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>131</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -6146,13 +6026,13 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>144</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -6166,7 +6046,7 @@
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>139</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -6180,7 +6060,7 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>138</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -6207,7 +6087,7 @@
         <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -6316,64 +6196,64 @@
         <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="E2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="H2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="I2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="J2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="K2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="M2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N2" t="s">
         <v>36</v>
       </c>
       <c r="O2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="P2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="Q2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="S2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="T2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U2" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -6381,64 +6261,64 @@
         <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="E3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="H3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="I3" t="s">
         <v>36</v>
       </c>
       <c r="J3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="K3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="M3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="O3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="P3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="Q3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="S3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="T3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -6446,64 +6326,64 @@
         <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F4" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G4" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="H4" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="I4" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="J4" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="K4" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L4" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="M4" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N4" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="O4" t="s">
         <v>36</v>
       </c>
       <c r="P4" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="Q4" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R4" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="S4" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="T4" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U4" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -6511,64 +6391,64 @@
         <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="E5" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F5" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G5" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="H5" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="I5" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="J5" t="s">
         <v>36</v>
       </c>
       <c r="K5" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L5" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="M5" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N5" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="O5" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="P5" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="Q5" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R5" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="S5" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="T5" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U5" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -6576,64 +6456,64 @@
         <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="E6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="H6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="I6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="J6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="K6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="M6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="O6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="P6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="Q6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="S6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="T6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U6" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -6641,61 +6521,61 @@
         <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="E7" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F7" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G7" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="H7" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="I7" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="J7" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="K7" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L7" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="M7" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N7" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="O7" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="P7" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="Q7" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R7" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="S7" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="T7" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U7" t="s">
         <v>36</v>
@@ -6706,64 +6586,64 @@
         <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="E8" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F8" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G8" t="s">
         <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="I8" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="J8" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="K8" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L8" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="M8" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N8" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="O8" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="P8" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="Q8" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R8" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="S8" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="T8" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U8" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -6771,61 +6651,61 @@
         <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C9" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D9" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="E9" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F9" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G9" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="H9" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="I9" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="J9" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="K9" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L9" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="M9" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N9" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="O9" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="P9" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="Q9" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R9" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="S9" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="T9" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U9" t="s">
         <v>36</v>
@@ -6836,64 +6716,64 @@
         <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="E10" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F10" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G10" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="H10" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="I10" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="J10" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="K10" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L10" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="M10" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N10" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="O10" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="P10" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="Q10" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R10" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="S10" t="s">
         <v>36</v>
       </c>
       <c r="T10" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U10" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -6901,64 +6781,64 @@
         <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
         <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="E11" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F11" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G11" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="H11" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="I11" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="J11" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="K11" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L11" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="M11" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N11" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="O11" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="P11" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="Q11" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R11" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="S11" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="T11" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U11" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -6966,64 +6846,64 @@
         <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C12" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D12" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="E12" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F12" t="s">
         <v>36</v>
       </c>
       <c r="G12" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="H12" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="I12" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="J12" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="K12" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L12" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="M12" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N12" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="O12" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="P12" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="Q12" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R12" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="S12" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="T12" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U12" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -7034,61 +6914,61 @@
         <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D13" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="E13" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F13" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G13" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="H13" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="I13" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="J13" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="K13" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L13" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="M13" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N13" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="O13" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="P13" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="Q13" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R13" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="S13" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="T13" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U13" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -7096,64 +6976,64 @@
         <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D14" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="E14" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F14" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G14" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="H14" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="I14" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="J14" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="K14" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L14" t="s">
         <v>36</v>
       </c>
       <c r="M14" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N14" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="O14" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="P14" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="Q14" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R14" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="S14" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="T14" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U14" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -7161,64 +7041,64 @@
         <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="E15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="H15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="I15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="J15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="K15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="M15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="O15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="P15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="Q15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="S15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="T15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U15" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -7226,64 +7106,64 @@
         <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
       </c>
       <c r="E16" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F16" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G16" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="H16" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="I16" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="J16" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="K16" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L16" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="M16" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N16" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="O16" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="P16" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="Q16" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R16" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="S16" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="T16" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U16" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -7291,64 +7171,64 @@
         <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="E17" t="s">
         <v>36</v>
       </c>
       <c r="F17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="H17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="I17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="J17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="K17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="M17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="O17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="P17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="Q17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="S17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="T17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -7356,64 +7236,64 @@
         <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="E18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="H18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="I18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="J18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="K18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="M18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="O18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="P18" t="s">
         <v>36</v>
       </c>
       <c r="Q18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="S18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="T18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U18" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -7421,64 +7301,64 @@
         <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D19" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="E19" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F19" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G19" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="H19" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="I19" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="J19" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="K19" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L19" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="M19" t="s">
         <v>36</v>
       </c>
       <c r="N19" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="O19" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="P19" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="Q19" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R19" t="s">
         <v>36</v>
       </c>
       <c r="S19" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="T19" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U19" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -7486,64 +7366,64 @@
         <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D20" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="E20" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F20" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G20" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="H20" t="s">
         <v>36</v>
       </c>
       <c r="I20" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="J20" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="K20" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L20" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="M20" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N20" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="O20" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="P20" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="Q20" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R20" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="S20" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="T20" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U20" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -7551,64 +7431,64 @@
         <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C21" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="D21" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="E21" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="F21" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G21" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="H21" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="I21" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="J21" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="K21" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="L21" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="M21" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N21" t="s">
         <v>36</v>
       </c>
       <c r="O21" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="P21" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="Q21" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R21" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="S21" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="T21" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="U21" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -7722,76 +7602,76 @@
         <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>119</v>
+        <v>79</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.25">
@@ -7799,76 +7679,76 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="J2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="L2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="N2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="P2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="R2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="T2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="V2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="X2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="Z2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AB2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AD2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AF2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AH2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AJ2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AL2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AN2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AP2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AR2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AT2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AV2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Dimensionless for nonstandard units, the actual units is set at attributes description
</commit_message>
<xml_diff>
--- a/data/Gas_Transmission/Gas_Trans.xlsx
+++ b/data/Gas_Transmission/Gas_Trans.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="111">
   <si>
     <t>Name</t>
   </si>
@@ -349,18 +349,9 @@
     <t>Arc flow (1e6 SCM)</t>
   </si>
   <si>
-    <t xml:space="preserve"> squared pressure</t>
-  </si>
-  <si>
     <t>supply cost</t>
   </si>
   <si>
-    <t>1e6*SCM</t>
-  </si>
-  <si>
-    <t>Volume</t>
-  </si>
-  <si>
     <t>Length</t>
   </si>
   <si>
@@ -370,12 +361,6 @@
     <t>mm</t>
   </si>
   <si>
-    <t>Energy price</t>
-  </si>
-  <si>
-    <t>USD MBTU^-1</t>
-  </si>
-  <si>
     <t>squared pressure</t>
   </si>
   <si>
@@ -383,6 +368,9 @@
   </si>
   <si>
     <t>Monetary value</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> squared pressure, 1e6*SCM</t>
   </si>
 </sst>
 </file>
@@ -714,7 +702,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,7 +753,7 @@
         <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4152,14 +4140,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
@@ -4225,10 +4212,10 @@
         <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>105</v>
+        <v>24</v>
       </c>
       <c r="K2" t="s">
         <v>24</v>
@@ -5015,7 +5002,6 @@
     <hyperlink ref="H15" location="pup!Z3" tooltip="Browse to 66.2" display="66.2"/>
     <hyperlink ref="I15" location="c!Z3" tooltip="Browse to 1.68" display="1.68"/>
     <hyperlink ref="H1" location="attributes!A10" tooltip="Browse to pup" display="pup"/>
-    <hyperlink ref="I1" location="attributes!A9" tooltip="Browse to c" display="c"/>
     <hyperlink ref="J1" location="attributes!A8" tooltip="Browse to s" display="s"/>
     <hyperlink ref="K1" location="attributes!A7" tooltip="Browse to pi" display="pi"/>
     <hyperlink ref="E15" location="slo!Z3" tooltip="Browse to 0" display="0"/>
@@ -5043,6 +5029,7 @@
     <hyperlink ref="H17" location="pup!AD3" tooltip="Browse to 63" display="63"/>
     <hyperlink ref="I17" location="c!AD3" tooltip="Browse to 0" display="0"/>
     <hyperlink ref="F12" location="sup!T3" tooltip="Browse to 4.8" display="4.8"/>
+    <hyperlink ref="I1" location="attributes!A9" tooltip="Browse to c" display="c"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5053,7 +5040,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5098,13 +5085,13 @@
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G2" t="s">
-        <v>105</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5736,7 +5723,6 @@
     <hyperlink ref="C15" location="nodes!A7" tooltip="Browse to Blaregnies" display="Blaregnies"/>
     <hyperlink ref="E15" location="D!Z3" tooltip="Browse to 890" display="890"/>
     <hyperlink ref="F15" location="L!Z3" tooltip="Browse to 25" display="25"/>
-    <hyperlink ref="E1" location="attributes!A6" tooltip="Browse to D" display="D"/>
     <hyperlink ref="F1" location="attributes!A5" tooltip="Browse to L" display="L"/>
     <hyperlink ref="G1" location="attributes!A4" tooltip="Browse to f" display="f"/>
     <hyperlink ref="B12" location="nodes!A11" tooltip="Browse to Liege" display="Liege"/>
@@ -5760,6 +5746,7 @@
     <hyperlink ref="E3" location="D!B3" tooltip="Browse to 890" display="890"/>
     <hyperlink ref="F3" location="L!B3" tooltip="Browse to 5" display="5"/>
     <hyperlink ref="C26" location="nodes!A15" tooltip="Browse to Peronnes" display="Peronnes"/>
+    <hyperlink ref="E1" location="attributes!A6" tooltip="Browse to D" display="D"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5828,14 +5815,14 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D34" sqref="D33:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="40.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5886,7 +5873,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -5900,7 +5887,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -5914,7 +5901,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -5934,7 +5921,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5942,13 +5929,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5956,7 +5943,7 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -6026,13 +6013,13 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>